<commit_message>
Changes to custom layout screen -- renamed to 'custom' and now uses field-name attr for placement.
</commit_message>
<xml_diff>
--- a/app/tables/gridScreen/forms/gridScreen/gridScreen.xlsx
+++ b/app/tables/gridScreen/forms/gridScreen/gridScreen.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="6360" windowWidth="29080" windowHeight="19520" tabRatio="439"/>
+    <workbookView xWindow="1920" yWindow="6360" windowWidth="25820" windowHeight="16220" tabRatio="439"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="127">
   <si>
     <t>type</t>
   </si>
@@ -222,18 +222,12 @@
     <t>display.image</t>
   </si>
   <si>
-    <t>screen_column</t>
-  </si>
-  <si>
     <t>screen.screen_type</t>
   </si>
   <si>
     <t>hideInContents</t>
   </si>
   <si>
-    <t>table_screen</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
@@ -397,17 +391,36 @@
   </si>
   <si>
     <t>Grid Screen Form</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>screen.templatePath</t>
+  </si>
+  <si>
+    <t>This is a test</t>
+  </si>
+  <si>
+    <t>../tables/gridScreen/forms/gridScreen/comparison_screen.handlebars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -448,14 +461,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -463,21 +476,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -785,31 +803,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="8" width="27.1640625" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" customWidth="1"/>
-    <col min="10" max="10" width="41.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.81640625" customWidth="1"/>
+    <col min="5" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="8" width="27.1796875" customWidth="1"/>
+    <col min="9" max="9" width="24.81640625" customWidth="1"/>
+    <col min="10" max="10" width="41.81640625" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" customWidth="1"/>
+    <col min="13" max="13" width="20.453125" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="17" width="18.5" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="16" max="17" width="18.453125" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
     <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" customWidth="1"/>
+    <col min="22" max="22" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17.5" customHeight="1">
+    <row r="1" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
         <v>60</v>
@@ -821,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="10" t="s">
         <v>66</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>0</v>
@@ -872,23 +890,25 @@
         <v>9</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="W1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17.5" customHeight="1">
+    <row r="2" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="4"/>
+        <v>123</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="5"/>
@@ -906,7 +926,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="17.5" customHeight="1">
+    <row r="3" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="D3" s="8"/>
@@ -917,13 +937,13 @@
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -937,7 +957,7 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:23" ht="17.5" customHeight="1">
+    <row r="4" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -945,11 +965,11 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="8"/>
@@ -965,10 +985,10 @@
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="17.5" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -976,11 +996,11 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="8"/>
@@ -996,10 +1016,10 @@
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
       <c r="W5" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="17.5" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1007,11 +1027,11 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="8"/>
@@ -1027,10 +1047,10 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="17.5" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1038,11 +1058,11 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="8"/>
@@ -1058,10 +1078,10 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="17.5" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1069,11 +1089,11 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="8"/>
@@ -1089,10 +1109,10 @@
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="17.5" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1100,11 +1120,11 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="8"/>
@@ -1120,10 +1140,10 @@
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
       <c r="W9" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="17.5" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1131,11 +1151,11 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="8"/>
@@ -1151,10 +1171,10 @@
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="17.5" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1166,7 +1186,7 @@
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="8"/>
@@ -1182,10 +1202,10 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="17.5" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1197,7 +1217,7 @@
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="8"/>
@@ -1213,10 +1233,10 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
       <c r="W12" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="17.5" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1228,7 +1248,7 @@
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="8"/>
@@ -1244,246 +1264,246 @@
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="17.5" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J14" s="12"/>
       <c r="W14" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="17.5" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J15" s="12"/>
       <c r="W15" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="17.5" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J16" s="12"/>
       <c r="W16" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G17" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J17" s="12"/>
       <c r="L17" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="W17" s="8"/>
     </row>
-    <row r="18" spans="3:23" ht="17.5" customHeight="1">
+    <row r="18" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J18" s="12"/>
       <c r="W18" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="3:23" ht="17.5" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J19" s="12"/>
       <c r="W19" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="3:23" ht="17.5" customHeight="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G20" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J20" s="12"/>
       <c r="W20" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="3:23" ht="17.5" customHeight="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G21" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J21" s="12"/>
       <c r="W21" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="3:23" ht="17.5" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G22" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J22" s="12"/>
       <c r="W22" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="3:23" ht="17.5" customHeight="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G23" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J23" s="12"/>
       <c r="W23" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="3:23" ht="17.5" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G24" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J24" s="12"/>
       <c r="W24" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G25" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J25" s="12"/>
       <c r="L25" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="W25" s="8"/>
     </row>
-    <row r="26" spans="3:23" ht="17.5" customHeight="1">
+    <row r="26" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G26" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J26" s="12"/>
       <c r="W26" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="3:23" ht="17.5" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J27" s="12"/>
       <c r="W27" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="3:23" ht="17.5" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G28" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J28" s="12"/>
       <c r="W28" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="3:23" ht="17.5" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G29" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J29" s="12"/>
       <c r="W29" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="3:23" ht="17.5" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G30" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J30" s="12"/>
       <c r="W30" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="3:23" ht="17.5" customHeight="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G31" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J31" s="12"/>
       <c r="W31" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="3:23" ht="17.5" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1493,32 +1513,32 @@
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J32" s="12"/>
       <c r="W32" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J33" s="12"/>
       <c r="L33" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W33" s="12"/>
     </row>
-    <row r="34" spans="3:23" ht="17.5" customHeight="1">
+    <row r="34" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1528,14 +1548,14 @@
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J34" s="12"/>
       <c r="W34" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="3:23" ht="17.5" customHeight="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1544,16 +1564,16 @@
         <v>59</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="3:23" ht="17.5" customHeight="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>15</v>
       </c>
@@ -1565,82 +1585,89 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="3:23" ht="17.5" customHeight="1">
-      <c r="C37" s="12"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="39" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="40" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="41" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="42" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="43" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="44" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="45" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="46" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="47" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="48" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="49" ht="17.5" customHeight="1"/>
-    <row r="50" ht="17.5" customHeight="1"/>
-    <row r="51" ht="17.5" customHeight="1"/>
-    <row r="52" ht="17.5" customHeight="1"/>
-    <row r="53" ht="17.5" customHeight="1"/>
-    <row r="54" ht="17.5" customHeight="1"/>
-    <row r="55" ht="17.5" customHeight="1"/>
-    <row r="56" ht="17.5" customHeight="1"/>
-    <row r="57" ht="17.5" customHeight="1"/>
-    <row r="58" ht="17.5" customHeight="1"/>
-    <row r="59" ht="17.5" customHeight="1"/>
-    <row r="60" ht="17.5" customHeight="1"/>
-    <row r="61" ht="17.5" customHeight="1"/>
-    <row r="62" ht="17.5" customHeight="1"/>
-    <row r="63" ht="17.5" customHeight="1"/>
-    <row r="64" ht="17.5" customHeight="1"/>
-    <row r="65" ht="17.5" customHeight="1"/>
-    <row r="66" ht="17.5" customHeight="1"/>
-    <row r="67" ht="17.5" customHeight="1"/>
-    <row r="68" ht="17.5" customHeight="1"/>
-    <row r="69" ht="17.5" customHeight="1"/>
-    <row r="70" ht="17.5" customHeight="1"/>
-    <row r="71" ht="17.5" customHeight="1"/>
-    <row r="72" ht="17.5" customHeight="1"/>
-    <row r="73" ht="17.5" customHeight="1"/>
-    <row r="74" ht="17.5" customHeight="1"/>
-    <row r="75" ht="17.5" customHeight="1"/>
-    <row r="76" ht="17.5" customHeight="1"/>
-    <row r="77" ht="17.5" customHeight="1"/>
-    <row r="78" ht="17.5" customHeight="1"/>
-    <row r="79" ht="17.5" customHeight="1"/>
-    <row r="80" ht="17.5" customHeight="1"/>
-    <row r="81" ht="17.5" customHeight="1"/>
-    <row r="82" ht="17.5" customHeight="1"/>
-    <row r="83" ht="17.5" customHeight="1"/>
-    <row r="84" ht="17.5" customHeight="1"/>
-    <row r="85" ht="17.5" customHeight="1"/>
-    <row r="86" ht="17.5" customHeight="1"/>
-    <row r="87" ht="17.5" customHeight="1"/>
-    <row r="88" ht="17.5" customHeight="1"/>
-    <row r="89" ht="17.5" customHeight="1"/>
-    <row r="90" ht="17.5" customHeight="1"/>
-    <row r="91" ht="17.5" customHeight="1"/>
-    <row r="92" ht="17.5" customHeight="1"/>
-    <row r="93" ht="17.5" customHeight="1"/>
-    <row r="94" ht="17.5" customHeight="1"/>
-    <row r="95" ht="17.5" customHeight="1"/>
-    <row r="96" ht="17.5" customHeight="1"/>
-    <row r="97" ht="17.5" customHeight="1"/>
-    <row r="98" ht="17.5" customHeight="1"/>
-    <row r="99" ht="17.5" customHeight="1"/>
-    <row r="100" ht="17.5" customHeight="1"/>
-    <row r="101" ht="17.5" customHeight="1"/>
-    <row r="102" ht="17.5" customHeight="1"/>
-    <row r="103" ht="17.5" customHeight="1"/>
-    <row r="104" ht="17.5" customHeight="1"/>
-    <row r="105" ht="17.5" customHeight="1"/>
-    <row r="106" ht="17.5" customHeight="1"/>
-    <row r="107" ht="17.5" customHeight="1"/>
+    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E37" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1659,13 +1686,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="1" max="1" width="25.6328125" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" customHeight="1">
+    <row r="1" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -1673,7 +1700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.5" customHeight="1">
+    <row r="2" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1681,28 +1708,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" customHeight="1">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1719,18 +1746,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" customHeight="1">
+    <row r="1" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1741,7 +1768,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.5" customHeight="1">
+    <row r="2" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1752,7 +1779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" customHeight="1">
+    <row r="3" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1763,7 +1790,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" customHeight="1">
+    <row r="4" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1774,7 +1801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" customHeight="1">
+    <row r="5" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1785,7 +1812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.5" customHeight="1">
+    <row r="6" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1796,7 +1823,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.5" customHeight="1">
+    <row r="7" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1807,7 +1834,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1">
+    <row r="8" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1818,7 +1845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.5" customHeight="1">
+    <row r="9" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1829,7 +1856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.5" customHeight="1">
+    <row r="10" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1840,8 +1867,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="12" spans="1:3" ht="17.5" customHeight="1">
+    <row r="11" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.5" customHeight="1">
+    <row r="13" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1863,7 +1890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.5" customHeight="1">
+    <row r="14" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1874,7 +1901,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.5" customHeight="1">
+    <row r="15" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1885,7 +1912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.5" customHeight="1">
+    <row r="16" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1896,7 +1923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" customHeight="1">
+    <row r="17" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1907,7 +1934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.5" customHeight="1">
+    <row r="18" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1918,7 +1945,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.5" customHeight="1">
+    <row r="19" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1929,7 +1956,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.5" customHeight="1">
+    <row r="20" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1940,7 +1967,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1">
+    <row r="21" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1951,8 +1978,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="23" spans="1:3" ht="17.5" customHeight="1">
+    <row r="22" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1963,7 +1990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.5" customHeight="1">
+    <row r="24" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1974,38 +2001,38 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="26" spans="1:3" ht="17.5" customHeight="1">
+    <row r="25" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A27" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A28" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="C28" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2026,14 +2053,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1">
+    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -2044,15 +2071,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" customHeight="1">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -2060,17 +2087,17 @@
         <v>20140227</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Changes to the custom screen - now named 'custom' and uses the field-name attr for placement.
</commit_message>
<xml_diff>
--- a/app/tables/gridScreen/forms/gridScreen/gridScreen.xlsx
+++ b/app/tables/gridScreen/forms/gridScreen/gridScreen.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="6360" windowWidth="29080" windowHeight="19520" tabRatio="439"/>
+    <workbookView xWindow="1920" yWindow="6360" windowWidth="25820" windowHeight="16220" tabRatio="439"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="127">
   <si>
     <t>type</t>
   </si>
@@ -222,18 +222,12 @@
     <t>display.image</t>
   </si>
   <si>
-    <t>screen_column</t>
-  </si>
-  <si>
     <t>screen.screen_type</t>
   </si>
   <si>
     <t>hideInContents</t>
   </si>
   <si>
-    <t>table_screen</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
@@ -397,17 +391,36 @@
   </si>
   <si>
     <t>Grid Screen Form</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>screen.templatePath</t>
+  </si>
+  <si>
+    <t>This is a test</t>
+  </si>
+  <si>
+    <t>../tables/gridScreen/forms/gridScreen/comparison_screen.handlebars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -448,14 +461,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -463,21 +476,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -785,31 +803,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="8" width="27.1640625" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" customWidth="1"/>
-    <col min="10" max="10" width="41.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.81640625" customWidth="1"/>
+    <col min="5" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="8" width="27.1796875" customWidth="1"/>
+    <col min="9" max="9" width="24.81640625" customWidth="1"/>
+    <col min="10" max="10" width="41.81640625" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" customWidth="1"/>
+    <col min="13" max="13" width="20.453125" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="17" width="18.5" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="16" max="17" width="18.453125" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
     <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" customWidth="1"/>
+    <col min="22" max="22" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17.5" customHeight="1">
+    <row r="1" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
         <v>60</v>
@@ -821,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="10" t="s">
         <v>66</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>0</v>
@@ -872,23 +890,25 @@
         <v>9</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="W1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17.5" customHeight="1">
+    <row r="2" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="4"/>
+        <v>123</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="5"/>
@@ -906,7 +926,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="17.5" customHeight="1">
+    <row r="3" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="D3" s="8"/>
@@ -917,13 +937,13 @@
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -937,7 +957,7 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:23" ht="17.5" customHeight="1">
+    <row r="4" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -945,11 +965,11 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="8"/>
@@ -965,10 +985,10 @@
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="17.5" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -976,11 +996,11 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="8"/>
@@ -996,10 +1016,10 @@
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
       <c r="W5" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="17.5" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1007,11 +1027,11 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="8"/>
@@ -1027,10 +1047,10 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="17.5" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1038,11 +1058,11 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="8"/>
@@ -1058,10 +1078,10 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="17.5" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1069,11 +1089,11 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="8"/>
@@ -1089,10 +1109,10 @@
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="17.5" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1100,11 +1120,11 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="8"/>
@@ -1120,10 +1140,10 @@
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
       <c r="W9" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="17.5" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1131,11 +1151,11 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="8"/>
@@ -1151,10 +1171,10 @@
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="17.5" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1166,7 +1186,7 @@
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="8"/>
@@ -1182,10 +1202,10 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="17.5" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1197,7 +1217,7 @@
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="8"/>
@@ -1213,10 +1233,10 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
       <c r="W12" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="17.5" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1228,7 +1248,7 @@
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="8"/>
@@ -1244,246 +1264,246 @@
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="17.5" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J14" s="12"/>
       <c r="W14" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="17.5" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J15" s="12"/>
       <c r="W15" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="17.5" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J16" s="12"/>
       <c r="W16" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G17" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J17" s="12"/>
       <c r="L17" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="W17" s="8"/>
     </row>
-    <row r="18" spans="3:23" ht="17.5" customHeight="1">
+    <row r="18" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J18" s="12"/>
       <c r="W18" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="3:23" ht="17.5" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J19" s="12"/>
       <c r="W19" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="3:23" ht="17.5" customHeight="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G20" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J20" s="12"/>
       <c r="W20" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="3:23" ht="17.5" customHeight="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G21" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J21" s="12"/>
       <c r="W21" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="3:23" ht="17.5" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G22" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J22" s="12"/>
       <c r="W22" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="3:23" ht="17.5" customHeight="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G23" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J23" s="12"/>
       <c r="W23" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="3:23" ht="17.5" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G24" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J24" s="12"/>
       <c r="W24" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G25" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J25" s="12"/>
       <c r="L25" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="W25" s="8"/>
     </row>
-    <row r="26" spans="3:23" ht="17.5" customHeight="1">
+    <row r="26" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G26" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J26" s="12"/>
       <c r="W26" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="3:23" ht="17.5" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J27" s="12"/>
       <c r="W27" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="3:23" ht="17.5" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G28" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J28" s="12"/>
       <c r="W28" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="3:23" ht="17.5" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G29" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J29" s="12"/>
       <c r="W29" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="3:23" ht="17.5" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G30" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J30" s="12"/>
       <c r="W30" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="3:23" ht="17.5" customHeight="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G31" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J31" s="12"/>
       <c r="W31" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="3:23" ht="17.5" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1493,32 +1513,32 @@
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J32" s="12"/>
       <c r="W32" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J33" s="12"/>
       <c r="L33" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W33" s="12"/>
     </row>
-    <row r="34" spans="3:23" ht="17.5" customHeight="1">
+    <row r="34" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1528,14 +1548,14 @@
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J34" s="12"/>
       <c r="W34" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="3:23" ht="17.5" customHeight="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1544,16 +1564,16 @@
         <v>59</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="3:23" ht="17.5" customHeight="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>15</v>
       </c>
@@ -1565,82 +1585,89 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="3:23" ht="17.5" customHeight="1">
-      <c r="C37" s="12"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="39" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="40" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="41" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="42" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="43" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="44" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="45" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="46" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="47" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="48" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="49" ht="17.5" customHeight="1"/>
-    <row r="50" ht="17.5" customHeight="1"/>
-    <row r="51" ht="17.5" customHeight="1"/>
-    <row r="52" ht="17.5" customHeight="1"/>
-    <row r="53" ht="17.5" customHeight="1"/>
-    <row r="54" ht="17.5" customHeight="1"/>
-    <row r="55" ht="17.5" customHeight="1"/>
-    <row r="56" ht="17.5" customHeight="1"/>
-    <row r="57" ht="17.5" customHeight="1"/>
-    <row r="58" ht="17.5" customHeight="1"/>
-    <row r="59" ht="17.5" customHeight="1"/>
-    <row r="60" ht="17.5" customHeight="1"/>
-    <row r="61" ht="17.5" customHeight="1"/>
-    <row r="62" ht="17.5" customHeight="1"/>
-    <row r="63" ht="17.5" customHeight="1"/>
-    <row r="64" ht="17.5" customHeight="1"/>
-    <row r="65" ht="17.5" customHeight="1"/>
-    <row r="66" ht="17.5" customHeight="1"/>
-    <row r="67" ht="17.5" customHeight="1"/>
-    <row r="68" ht="17.5" customHeight="1"/>
-    <row r="69" ht="17.5" customHeight="1"/>
-    <row r="70" ht="17.5" customHeight="1"/>
-    <row r="71" ht="17.5" customHeight="1"/>
-    <row r="72" ht="17.5" customHeight="1"/>
-    <row r="73" ht="17.5" customHeight="1"/>
-    <row r="74" ht="17.5" customHeight="1"/>
-    <row r="75" ht="17.5" customHeight="1"/>
-    <row r="76" ht="17.5" customHeight="1"/>
-    <row r="77" ht="17.5" customHeight="1"/>
-    <row r="78" ht="17.5" customHeight="1"/>
-    <row r="79" ht="17.5" customHeight="1"/>
-    <row r="80" ht="17.5" customHeight="1"/>
-    <row r="81" ht="17.5" customHeight="1"/>
-    <row r="82" ht="17.5" customHeight="1"/>
-    <row r="83" ht="17.5" customHeight="1"/>
-    <row r="84" ht="17.5" customHeight="1"/>
-    <row r="85" ht="17.5" customHeight="1"/>
-    <row r="86" ht="17.5" customHeight="1"/>
-    <row r="87" ht="17.5" customHeight="1"/>
-    <row r="88" ht="17.5" customHeight="1"/>
-    <row r="89" ht="17.5" customHeight="1"/>
-    <row r="90" ht="17.5" customHeight="1"/>
-    <row r="91" ht="17.5" customHeight="1"/>
-    <row r="92" ht="17.5" customHeight="1"/>
-    <row r="93" ht="17.5" customHeight="1"/>
-    <row r="94" ht="17.5" customHeight="1"/>
-    <row r="95" ht="17.5" customHeight="1"/>
-    <row r="96" ht="17.5" customHeight="1"/>
-    <row r="97" ht="17.5" customHeight="1"/>
-    <row r="98" ht="17.5" customHeight="1"/>
-    <row r="99" ht="17.5" customHeight="1"/>
-    <row r="100" ht="17.5" customHeight="1"/>
-    <row r="101" ht="17.5" customHeight="1"/>
-    <row r="102" ht="17.5" customHeight="1"/>
-    <row r="103" ht="17.5" customHeight="1"/>
-    <row r="104" ht="17.5" customHeight="1"/>
-    <row r="105" ht="17.5" customHeight="1"/>
-    <row r="106" ht="17.5" customHeight="1"/>
-    <row r="107" ht="17.5" customHeight="1"/>
+    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E37" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1659,13 +1686,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="1" max="1" width="25.6328125" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" customHeight="1">
+    <row r="1" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -1673,7 +1700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.5" customHeight="1">
+    <row r="2" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1681,28 +1708,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" customHeight="1">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1719,18 +1746,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" customHeight="1">
+    <row r="1" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1741,7 +1768,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.5" customHeight="1">
+    <row r="2" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1752,7 +1779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" customHeight="1">
+    <row r="3" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1763,7 +1790,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" customHeight="1">
+    <row r="4" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1774,7 +1801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" customHeight="1">
+    <row r="5" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1785,7 +1812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.5" customHeight="1">
+    <row r="6" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1796,7 +1823,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.5" customHeight="1">
+    <row r="7" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1807,7 +1834,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1">
+    <row r="8" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1818,7 +1845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.5" customHeight="1">
+    <row r="9" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1829,7 +1856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.5" customHeight="1">
+    <row r="10" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1840,8 +1867,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="12" spans="1:3" ht="17.5" customHeight="1">
+    <row r="11" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.5" customHeight="1">
+    <row r="13" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1863,7 +1890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.5" customHeight="1">
+    <row r="14" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1874,7 +1901,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.5" customHeight="1">
+    <row r="15" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1885,7 +1912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.5" customHeight="1">
+    <row r="16" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1896,7 +1923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" customHeight="1">
+    <row r="17" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1907,7 +1934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.5" customHeight="1">
+    <row r="18" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1918,7 +1945,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.5" customHeight="1">
+    <row r="19" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1929,7 +1956,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.5" customHeight="1">
+    <row r="20" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1940,7 +1967,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1">
+    <row r="21" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1951,8 +1978,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="23" spans="1:3" ht="17.5" customHeight="1">
+    <row r="22" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1963,7 +1990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.5" customHeight="1">
+    <row r="24" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1974,38 +2001,38 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="26" spans="1:3" ht="17.5" customHeight="1">
+    <row r="25" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A27" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A28" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="C28" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2026,14 +2053,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1">
+    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -2044,15 +2071,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" customHeight="1">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -2060,17 +2087,17 @@
         <v>20140227</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Changes to custom screen - now named 'custom' and uses the field-name attr for placements.
</commit_message>
<xml_diff>
--- a/app/tables/gridScreen/forms/gridScreen/gridScreen.xlsx
+++ b/app/tables/gridScreen/forms/gridScreen/gridScreen.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="6360" windowWidth="29080" windowHeight="19520" tabRatio="439"/>
+    <workbookView xWindow="1920" yWindow="6360" windowWidth="25820" windowHeight="16220" tabRatio="439"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="127">
   <si>
     <t>type</t>
   </si>
@@ -222,18 +222,12 @@
     <t>display.image</t>
   </si>
   <si>
-    <t>screen_column</t>
-  </si>
-  <si>
     <t>screen.screen_type</t>
   </si>
   <si>
     <t>hideInContents</t>
   </si>
   <si>
-    <t>table_screen</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
@@ -397,17 +391,36 @@
   </si>
   <si>
     <t>Grid Screen Form</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>screen.templatePath</t>
+  </si>
+  <si>
+    <t>This is a test</t>
+  </si>
+  <si>
+    <t>../tables/gridScreen/forms/gridScreen/comparison_screen.handlebars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -448,14 +461,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -463,21 +476,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -785,31 +803,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="8" width="27.1640625" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" customWidth="1"/>
-    <col min="10" max="10" width="41.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.81640625" customWidth="1"/>
+    <col min="5" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="8" width="27.1796875" customWidth="1"/>
+    <col min="9" max="9" width="24.81640625" customWidth="1"/>
+    <col min="10" max="10" width="41.81640625" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" customWidth="1"/>
+    <col min="13" max="13" width="20.453125" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="17" width="18.5" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="16" max="17" width="18.453125" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
     <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" customWidth="1"/>
+    <col min="22" max="22" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17.5" customHeight="1">
+    <row r="1" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
         <v>60</v>
@@ -821,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="10" t="s">
         <v>66</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>0</v>
@@ -872,23 +890,25 @@
         <v>9</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="W1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17.5" customHeight="1">
+    <row r="2" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="4"/>
+        <v>123</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="5"/>
@@ -906,7 +926,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="17.5" customHeight="1">
+    <row r="3" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="D3" s="8"/>
@@ -917,13 +937,13 @@
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -937,7 +957,7 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:23" ht="17.5" customHeight="1">
+    <row r="4" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -945,11 +965,11 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="8"/>
@@ -965,10 +985,10 @@
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="17.5" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -976,11 +996,11 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="8"/>
@@ -996,10 +1016,10 @@
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
       <c r="W5" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="17.5" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1007,11 +1027,11 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="8"/>
@@ -1027,10 +1047,10 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="17.5" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1038,11 +1058,11 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="8"/>
@@ -1058,10 +1078,10 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="17.5" customHeight="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1069,11 +1089,11 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="8"/>
@@ -1089,10 +1109,10 @@
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="17.5" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1100,11 +1120,11 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="8"/>
@@ -1120,10 +1140,10 @@
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
       <c r="W9" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="17.5" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1131,11 +1151,11 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="8"/>
@@ -1151,10 +1171,10 @@
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="17.5" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1166,7 +1186,7 @@
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="8"/>
@@ -1182,10 +1202,10 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="17.5" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1197,7 +1217,7 @@
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="8"/>
@@ -1213,10 +1233,10 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
       <c r="W12" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="17.5" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1228,7 +1248,7 @@
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="8"/>
@@ -1244,246 +1264,246 @@
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="17.5" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J14" s="12"/>
       <c r="W14" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="17.5" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J15" s="12"/>
       <c r="W15" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="17.5" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J16" s="12"/>
       <c r="W16" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G17" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J17" s="12"/>
       <c r="L17" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="W17" s="8"/>
     </row>
-    <row r="18" spans="3:23" ht="17.5" customHeight="1">
+    <row r="18" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J18" s="12"/>
       <c r="W18" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="3:23" ht="17.5" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J19" s="12"/>
       <c r="W19" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="3:23" ht="17.5" customHeight="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G20" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J20" s="12"/>
       <c r="W20" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="3:23" ht="17.5" customHeight="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G21" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J21" s="12"/>
       <c r="W21" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="3:23" ht="17.5" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G22" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J22" s="12"/>
       <c r="W22" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="3:23" ht="17.5" customHeight="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G23" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J23" s="12"/>
       <c r="W23" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="3:23" ht="17.5" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G24" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J24" s="12"/>
       <c r="W24" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G25" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J25" s="12"/>
       <c r="L25" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="W25" s="8"/>
     </row>
-    <row r="26" spans="3:23" ht="17.5" customHeight="1">
+    <row r="26" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G26" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J26" s="12"/>
       <c r="W26" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="3:23" ht="17.5" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J27" s="12"/>
       <c r="W27" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="3:23" ht="17.5" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G28" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J28" s="12"/>
       <c r="W28" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="3:23" ht="17.5" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G29" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J29" s="12"/>
       <c r="W29" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="3:23" ht="17.5" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G30" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J30" s="12"/>
       <c r="W30" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="3:23" ht="17.5" customHeight="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G31" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J31" s="12"/>
       <c r="W31" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="3:23" ht="17.5" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1493,32 +1513,32 @@
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J32" s="12"/>
       <c r="W32" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J33" s="12"/>
       <c r="L33" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W33" s="12"/>
     </row>
-    <row r="34" spans="3:23" ht="17.5" customHeight="1">
+    <row r="34" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1528,14 +1548,14 @@
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J34" s="12"/>
       <c r="W34" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="3:23" ht="17.5" customHeight="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1544,16 +1564,16 @@
         <v>59</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="3:23" ht="17.5" customHeight="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>15</v>
       </c>
@@ -1565,82 +1585,89 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="3:23" ht="17.5" customHeight="1">
-      <c r="C37" s="12"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="39" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="40" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="41" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="42" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="43" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="44" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="45" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="46" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="47" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="48" spans="3:23" ht="17.5" customHeight="1"/>
-    <row r="49" ht="17.5" customHeight="1"/>
-    <row r="50" ht="17.5" customHeight="1"/>
-    <row r="51" ht="17.5" customHeight="1"/>
-    <row r="52" ht="17.5" customHeight="1"/>
-    <row r="53" ht="17.5" customHeight="1"/>
-    <row r="54" ht="17.5" customHeight="1"/>
-    <row r="55" ht="17.5" customHeight="1"/>
-    <row r="56" ht="17.5" customHeight="1"/>
-    <row r="57" ht="17.5" customHeight="1"/>
-    <row r="58" ht="17.5" customHeight="1"/>
-    <row r="59" ht="17.5" customHeight="1"/>
-    <row r="60" ht="17.5" customHeight="1"/>
-    <row r="61" ht="17.5" customHeight="1"/>
-    <row r="62" ht="17.5" customHeight="1"/>
-    <row r="63" ht="17.5" customHeight="1"/>
-    <row r="64" ht="17.5" customHeight="1"/>
-    <row r="65" ht="17.5" customHeight="1"/>
-    <row r="66" ht="17.5" customHeight="1"/>
-    <row r="67" ht="17.5" customHeight="1"/>
-    <row r="68" ht="17.5" customHeight="1"/>
-    <row r="69" ht="17.5" customHeight="1"/>
-    <row r="70" ht="17.5" customHeight="1"/>
-    <row r="71" ht="17.5" customHeight="1"/>
-    <row r="72" ht="17.5" customHeight="1"/>
-    <row r="73" ht="17.5" customHeight="1"/>
-    <row r="74" ht="17.5" customHeight="1"/>
-    <row r="75" ht="17.5" customHeight="1"/>
-    <row r="76" ht="17.5" customHeight="1"/>
-    <row r="77" ht="17.5" customHeight="1"/>
-    <row r="78" ht="17.5" customHeight="1"/>
-    <row r="79" ht="17.5" customHeight="1"/>
-    <row r="80" ht="17.5" customHeight="1"/>
-    <row r="81" ht="17.5" customHeight="1"/>
-    <row r="82" ht="17.5" customHeight="1"/>
-    <row r="83" ht="17.5" customHeight="1"/>
-    <row r="84" ht="17.5" customHeight="1"/>
-    <row r="85" ht="17.5" customHeight="1"/>
-    <row r="86" ht="17.5" customHeight="1"/>
-    <row r="87" ht="17.5" customHeight="1"/>
-    <row r="88" ht="17.5" customHeight="1"/>
-    <row r="89" ht="17.5" customHeight="1"/>
-    <row r="90" ht="17.5" customHeight="1"/>
-    <row r="91" ht="17.5" customHeight="1"/>
-    <row r="92" ht="17.5" customHeight="1"/>
-    <row r="93" ht="17.5" customHeight="1"/>
-    <row r="94" ht="17.5" customHeight="1"/>
-    <row r="95" ht="17.5" customHeight="1"/>
-    <row r="96" ht="17.5" customHeight="1"/>
-    <row r="97" ht="17.5" customHeight="1"/>
-    <row r="98" ht="17.5" customHeight="1"/>
-    <row r="99" ht="17.5" customHeight="1"/>
-    <row r="100" ht="17.5" customHeight="1"/>
-    <row r="101" ht="17.5" customHeight="1"/>
-    <row r="102" ht="17.5" customHeight="1"/>
-    <row r="103" ht="17.5" customHeight="1"/>
-    <row r="104" ht="17.5" customHeight="1"/>
-    <row r="105" ht="17.5" customHeight="1"/>
-    <row r="106" ht="17.5" customHeight="1"/>
-    <row r="107" ht="17.5" customHeight="1"/>
+    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E37" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="3:23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1659,13 +1686,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="1" max="1" width="25.6328125" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" customHeight="1">
+    <row r="1" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -1673,7 +1700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.5" customHeight="1">
+    <row r="2" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1681,28 +1708,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" customHeight="1">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1719,18 +1746,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" customHeight="1">
+    <row r="1" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1741,7 +1768,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.5" customHeight="1">
+    <row r="2" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1752,7 +1779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" customHeight="1">
+    <row r="3" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1763,7 +1790,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" customHeight="1">
+    <row r="4" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1774,7 +1801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" customHeight="1">
+    <row r="5" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1785,7 +1812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.5" customHeight="1">
+    <row r="6" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1796,7 +1823,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.5" customHeight="1">
+    <row r="7" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1807,7 +1834,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1">
+    <row r="8" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1818,7 +1845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.5" customHeight="1">
+    <row r="9" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1829,7 +1856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.5" customHeight="1">
+    <row r="10" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1840,8 +1867,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="12" spans="1:3" ht="17.5" customHeight="1">
+    <row r="11" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.5" customHeight="1">
+    <row r="13" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1863,7 +1890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.5" customHeight="1">
+    <row r="14" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1874,7 +1901,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.5" customHeight="1">
+    <row r="15" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1885,7 +1912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.5" customHeight="1">
+    <row r="16" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1896,7 +1923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" customHeight="1">
+    <row r="17" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1907,7 +1934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.5" customHeight="1">
+    <row r="18" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1918,7 +1945,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.5" customHeight="1">
+    <row r="19" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1929,7 +1956,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.5" customHeight="1">
+    <row r="20" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1940,7 +1967,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1">
+    <row r="21" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1951,8 +1978,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="23" spans="1:3" ht="17.5" customHeight="1">
+    <row r="22" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1963,7 +1990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.5" customHeight="1">
+    <row r="24" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1974,38 +2001,38 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="26" spans="1:3" ht="17.5" customHeight="1">
+    <row r="25" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A27" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A28" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="C28" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2026,14 +2053,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1">
+    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
@@ -2044,15 +2071,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" customHeight="1">
+    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -2060,17 +2087,17 @@
         <v>20140227</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>